<commit_message>
project cleaning, hotelname normalizer refined, new built in updateMode (not ready yet), hotelNameMapper refined
</commit_message>
<xml_diff>
--- a/puppeteer-server/assets/UAE_MatchedHotels.xlsx
+++ b/puppeteer-server/assets/UAE_MatchedHotels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27718"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27723"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asimov\Desktop\develop\hotelsScraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asimov\Desktop\cws_1.4.3\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C8193F-9469-42C2-AE93-BC20A1B01A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351B1BA4-9F49-418C-B2C2-83E627510F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,9 +856,6 @@
     <t>address boulevard *****</t>
   </si>
   <si>
-    <t>address boulevard dubai hotel *****</t>
-  </si>
-  <si>
     <t>kempinski central avenue dubai*****</t>
   </si>
   <si>
@@ -1202,13 +1199,16 @@
   </si>
   <si>
     <t>MERCURE HOTELS SUITES APARTMENTS, BARSHA HEIGHTS Hotel Apartments Standard</t>
+  </si>
+  <si>
+    <t>KEMPINSKI THE BOULEVARD DUBAI *****</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1249,6 +1249,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1331,7 +1337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1345,6 +1351,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1686,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1738,7 +1745,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -1832,7 +1839,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1880,7 +1887,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>35</v>
@@ -1917,7 +1924,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1925,7 +1932,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>43</v>
@@ -1934,7 +1941,7 @@
         <v>43</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1968,7 +1975,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1999,7 +2006,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>58</v>
@@ -2027,7 +2034,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>62</v>
@@ -2036,7 +2043,7 @@
         <v>63</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2044,16 +2051,16 @@
         <v>64</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>378</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2067,7 +2074,7 @@
         <v>67</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>68</v>
@@ -2078,16 +2085,16 @@
         <v>69</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>354</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>355</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2138,7 +2145,7 @@
         <v>81</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2274,7 +2281,7 @@
         <v>102</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2325,7 +2332,7 @@
         <v>109</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2410,7 +2417,7 @@
         <v>125</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -2486,7 +2493,7 @@
         <v>145</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>146</v>
@@ -2506,7 +2513,7 @@
         <v>149</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>150</v>
@@ -2557,13 +2564,13 @@
         <v>158</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>158</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2591,10 +2598,10 @@
         <v>164</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>163</v>
@@ -2628,7 +2635,7 @@
         <v>170</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>171</v>
@@ -2639,16 +2646,16 @@
         <v>172</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>173</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2696,7 +2703,7 @@
         <v>184</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>185</v>
@@ -2750,7 +2757,7 @@
         <v>196</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2758,7 +2765,7 @@
         <v>197</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>198</v>
@@ -2784,7 +2791,7 @@
         <v>204</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2795,13 +2802,13 @@
         <v>206</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>207</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2832,10 +2839,10 @@
         <v>212</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>386</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2852,7 +2859,7 @@
         <v>214</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2869,7 +2876,7 @@
         <v>217</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2877,13 +2884,13 @@
         <v>218</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>219</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>220</v>
@@ -2894,13 +2901,13 @@
         <v>221</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>222</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>223</v>
@@ -2937,7 +2944,7 @@
         <v>228</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2993,7 +3000,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>239</v>
@@ -3002,7 +3009,7 @@
         <v>240</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>241</v>
@@ -3016,13 +3023,13 @@
         <v>243</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D78" t="s">
         <v>243</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -3138,7 +3145,7 @@
         <v>262</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>263</v>
@@ -3200,441 +3207,441 @@
         <v>277</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="D89" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>278</v>
+      <c r="E89" s="11" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="C90" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" t="s">
+        <v>281</v>
+      </c>
+      <c r="D91" t="s">
+        <v>281</v>
+      </c>
+      <c r="E91" s="9" t="s">
         <v>282</v>
-      </c>
-      <c r="C91" t="s">
-        <v>282</v>
-      </c>
-      <c r="D91" t="s">
-        <v>282</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D92" t="s">
         <v>284</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="D92" t="s">
-        <v>285</v>
-      </c>
       <c r="E92" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D93" t="s">
         <v>287</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="D93" t="s">
-        <v>288</v>
-      </c>
       <c r="E93" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="C99" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="E100" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="C101" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="E103" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D104" s="2" t="s">
+      <c r="E104" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" t="s">
         <v>324</v>
       </c>
-      <c r="D105" t="s">
-        <v>325</v>
-      </c>
       <c r="E105" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="D106" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>330</v>
-      </c>
       <c r="D107" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="D108" t="s">
         <v>333</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" s="9" t="s">
         <v>334</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D109" t="s">
+        <v>336</v>
+      </c>
+      <c r="E109" s="9" t="s">
         <v>337</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="D109" t="s">
-        <v>337</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D110" t="s">
+        <v>339</v>
+      </c>
+      <c r="E110" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D110" t="s">
-        <v>340</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D111" t="s">
         <v>343</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D111" t="s">
-        <v>344</v>
-      </c>
       <c r="E111" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D112" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="D113" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B114" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C114" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D114" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E114" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test browser left open for debugging, last page not being scraped bug fixed
</commit_message>
<xml_diff>
--- a/puppeteer-server/assets/UAE_MatchedHotels.xlsx
+++ b/puppeteer-server/assets/UAE_MatchedHotels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asimov\Desktop\cws_1.4.3\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asimov\Desktop\develop\webscraper\puppeteer-server\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351B1BA4-9F49-418C-B2C2-83E627510F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEA3D1D-E355-4ACF-AD87-265B431910F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>riviera hotel ****</t>
   </si>
   <si>
-    <t>riviera dubai 4*</t>
-  </si>
-  <si>
     <t>millennium place barsha heights 4*</t>
   </si>
   <si>
@@ -1202,6 +1199,9 @@
   </si>
   <si>
     <t>KEMPINSKI THE BOULEVARD DUBAI *****</t>
+  </si>
+  <si>
+    <t>riviera hotel 4*</t>
   </si>
 </sst>
 </file>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1745,10 +1745,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>393</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1759,1895 +1759,1895 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>377</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E26" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="E39" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E48" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="C51" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C53" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="E62" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="E64" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="E65" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="D66" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="C67" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="C68" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="E69" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="C72" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="C73" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="D76" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C77" t="s">
         <v>239</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>240</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="C78" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D78" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E79" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="E84" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" t="s">
+        <v>261</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E85" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="C85" t="s">
-        <v>262</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" t="s">
         <v>266</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>263</v>
+      </c>
+      <c r="E86" s="9" t="s">
         <v>267</v>
-      </c>
-      <c r="D86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" t="s">
         <v>270</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>270</v>
+      </c>
+      <c r="E87" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="D87" t="s">
-        <v>271</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" t="s">
         <v>274</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
+        <v>273</v>
+      </c>
+      <c r="E88" s="9" t="s">
         <v>275</v>
-      </c>
-      <c r="D88" t="s">
-        <v>274</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="D89" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>367</v>
-      </c>
       <c r="E89" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="C90" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" t="s">
+        <v>280</v>
+      </c>
+      <c r="D91" t="s">
+        <v>280</v>
+      </c>
+      <c r="E91" s="9" t="s">
         <v>281</v>
-      </c>
-      <c r="C91" t="s">
-        <v>281</v>
-      </c>
-      <c r="D91" t="s">
-        <v>281</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D92" t="s">
         <v>283</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D92" t="s">
-        <v>284</v>
-      </c>
       <c r="E92" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D93" t="s">
         <v>286</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="D93" t="s">
-        <v>287</v>
-      </c>
       <c r="E93" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="C99" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="E100" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>310</v>
-      </c>
       <c r="C101" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="E103" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D104" s="2" t="s">
+      <c r="E104" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" t="s">
         <v>323</v>
       </c>
-      <c r="D105" t="s">
-        <v>324</v>
-      </c>
       <c r="E105" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="D106" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="D107" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="D108" t="s">
         <v>332</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D109" t="s">
+        <v>335</v>
+      </c>
+      <c r="E109" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D109" t="s">
-        <v>336</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D110" t="s">
+        <v>338</v>
+      </c>
+      <c r="E110" s="9" t="s">
         <v>339</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="D110" t="s">
-        <v>339</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D111" t="s">
         <v>342</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D111" t="s">
-        <v>343</v>
-      </c>
       <c r="E111" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D112" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>348</v>
-      </c>
       <c r="D113" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A2:E2 A24:E25 A60:E61 A62:D62 A69:D69 A105:A106 A107:C109 A113:E113 A68:D68 A4:E7 A3 C3:E3 A15:E15 A14 C14:D14 A22:C22 A20:A21 C20:D20 A23 D23 A49:E50 A47 C47:E47 A48:B48 D48:E48 A52:E52 A51:B51 D51 A54:E54 A53:B53 E53 A57:E58 A56 C56 A64:D64 A63 C63:E63 A66:E66 A65:B65 D65 A72:E72 A70:A71 C70:C71 A79:E84 B77 A78:B78 A91:B91 A89 A90:B90 A94:E99 A92 A93:B93 A101:E104 A100 C100:E100 C105 C106 A114:E114 A12:E12 A11:C11 E11 A9:E10 A8:D8 A13:D13 A17:E17 A16:D16 A27:E33 A26:D26 A19:E19 A18:C18 E18 E22 A35:E36 A38:E41 A37:D37 A43:E46 A42:D42 A55:C55 E55 A59:C59 E59 A67:C67 E70:E71 A74:E76 A73:D73 A85:B88 A110:C112" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 A2:E2 A24:E25 A60:E61 A62:D62 A69:D69 A105:A106 A107:C109 A113:E113 A68:D68 A4:E6 A3 D3:E3 A15:E15 A14 C14:D14 A22:C22 A20:A21 C20:D20 A23 D23 A49:E50 A47 C47:E47 A48:B48 D48:E48 A52:E52 A51:B51 D51 A54:E54 A53:B53 E53 A57:E58 A56 C56 A64:D64 A63 C63:E63 A66:E66 A65:B65 D65 A72:E72 A70:A71 C70:C71 A79:E84 B77 A78:B78 A91:B91 A89 A90:B90 A94:E99 A92 A93:B93 A101:E104 A100 C100:E100 C105 C106 A114:E114 A12:E12 A11:C11 E11 A9:E10 A8:D8 A13:D13 A17:E17 A16:D16 A27:E33 A26:D26 A19:E19 A18:C18 E18 E22 A35:E36 A38:E41 A37:D37 A43:E46 A42:D42 A55:C55 E55 A59:C59 E59 A67:C67 E70:E71 A74:E76 A73:D73 A85:B88 A110:C112 A7:B7 D7:E7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated hotel mappings to reflect the actual names
</commit_message>
<xml_diff>
--- a/puppeteer-server/assets/UAE_MatchedHotels.xlsx
+++ b/puppeteer-server/assets/UAE_MatchedHotels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27806"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asimov\Desktop\develop\webscraper\puppeteer-server\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEA3D1D-E355-4ACF-AD87-265B431910F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DA7C3C-9F34-493C-889F-B75A1C4D83F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="352">
   <si>
     <t>Online Centrum</t>
   </si>
@@ -58,9 +58,6 @@
     <t>millennium place barsha heights ****</t>
   </si>
   <si>
-    <t>hyatt place dubai/wasl district ****</t>
-  </si>
-  <si>
     <t>hyatt place dubai wasl district 4*</t>
   </si>
   <si>
@@ -70,18 +67,12 @@
     <t>copthorne hotel dubai 4*</t>
   </si>
   <si>
-    <t>copthorne hotel dubai. ****</t>
-  </si>
-  <si>
     <t>copthorne hotel dubai ****</t>
   </si>
   <si>
     <t>citymax bur dubai 3*</t>
   </si>
   <si>
-    <t>citymax bur dubai ***</t>
-  </si>
-  <si>
     <t>citymax hotel bur dubai 3*</t>
   </si>
   <si>
@@ -91,15 +82,9 @@
     <t>flora al barsha 4*</t>
   </si>
   <si>
-    <t>flora al barsha ****</t>
-  </si>
-  <si>
     <t>flora al barsha hotel 4*</t>
   </si>
   <si>
-    <t>rove dubai marina hotel ***</t>
-  </si>
-  <si>
     <t>rove dubai marina 3*</t>
   </si>
   <si>
@@ -115,9 +100,6 @@
     <t>citymax business bay 4*</t>
   </si>
   <si>
-    <t>fortune grand hotel. ****</t>
-  </si>
-  <si>
     <t>fortune grand hotel 4*</t>
   </si>
   <si>
@@ -136,24 +118,15 @@
     <t>lemon tree hotel 4*</t>
   </si>
   <si>
-    <t>novotel dubai al barsha. ****</t>
-  </si>
-  <si>
     <t>novotel dubai al barsha 4*</t>
   </si>
   <si>
     <t>novotel al barsha 4*</t>
   </si>
   <si>
-    <t>comfort inn hotel. ***</t>
-  </si>
-  <si>
     <t>comfort inn 3*</t>
   </si>
   <si>
-    <t>best western plus pearl creek hotel. ****</t>
-  </si>
-  <si>
     <t>best western plus pearl creek hotel 4*</t>
   </si>
   <si>
@@ -163,9 +136,6 @@
     <t>best western plus pearl creek hotel ****</t>
   </si>
   <si>
-    <t>ibis al barsha dubai ***</t>
-  </si>
-  <si>
     <t>ibis al barsha 3*</t>
   </si>
   <si>
@@ -175,18 +145,12 @@
     <t>the s hotel al barsha, dubai ****</t>
   </si>
   <si>
-    <t>aloft al mina ****</t>
-  </si>
-  <si>
     <t>aloft al mina 4*</t>
   </si>
   <si>
     <t>aloft al mina, dubai ****</t>
   </si>
   <si>
-    <t>city avenue hotel ***</t>
-  </si>
-  <si>
     <t>city avenue hotel 3*</t>
   </si>
   <si>
@@ -202,21 +166,12 @@
     <t>arabian park edge by rotana 3*</t>
   </si>
   <si>
-    <t>studio m arabian plaza hotel apartment ***</t>
-  </si>
-  <si>
     <t>studio m arabian plaza hotel &amp; apartments 3*</t>
   </si>
   <si>
     <t>studio m arabian plaza hotel &amp; hotel apartments 3*</t>
   </si>
   <si>
-    <t>md hotel dubai ****</t>
-  </si>
-  <si>
-    <t>grand excelsior bur dubai. ****</t>
-  </si>
-  <si>
     <t>grand excelsior hotel bur dubai 4*</t>
   </si>
   <si>
@@ -226,9 +181,6 @@
     <t>grand excelsior hotel bur dubai ****</t>
   </si>
   <si>
-    <t>rose park al barsha ****</t>
-  </si>
-  <si>
     <t>rose park al barsha 4*</t>
   </si>
   <si>
@@ -241,9 +193,6 @@
     <t>millennium central downtown 4*</t>
   </si>
   <si>
-    <t>al khoory executive. ***</t>
-  </si>
-  <si>
     <t>al khoory executive hotel 3*</t>
   </si>
   <si>
@@ -253,9 +202,6 @@
     <t>al khoory executive hotel ****</t>
   </si>
   <si>
-    <t>damac hills 2 hotel edge by rotana ***</t>
-  </si>
-  <si>
     <t>damac hills 2 hotel, an edge by rotana hotel 3*</t>
   </si>
   <si>
@@ -274,33 +220,21 @@
     <t>rose rayhaan by rotana 4*</t>
   </si>
   <si>
-    <t>rose rayhaan by rotana. ****</t>
-  </si>
-  <si>
     <t>rose rayhaan by rotana ****</t>
   </si>
   <si>
     <t>hyatt place dubai baniyas square 4*</t>
   </si>
   <si>
-    <t>hyatt place dubai baniyas square ****</t>
-  </si>
-  <si>
     <t>hyatt place dubai / baniyas square ****</t>
   </si>
   <si>
-    <t>hyatt place dubai/ al rigga ****</t>
-  </si>
-  <si>
     <t>hyatt place dubai al rigga 4*</t>
   </si>
   <si>
     <t>hyatt place dubai / al rigga ****</t>
   </si>
   <si>
-    <t>delta hotels by marriott, jumeirah beach dubai ****</t>
-  </si>
-  <si>
     <t>delta hotels by marriott jumeirah beach 4*</t>
   </si>
   <si>
@@ -316,9 +250,6 @@
     <t>riu dubai ****</t>
   </si>
   <si>
-    <t>centara mirage beach dubai ****</t>
-  </si>
-  <si>
     <t>centara mirage beach resort dubai 4*</t>
   </si>
   <si>
@@ -328,9 +259,6 @@
     <t>swissotel al ghurair dubai 5*</t>
   </si>
   <si>
-    <t>swissotel al ghurair dubai *****</t>
-  </si>
-  <si>
     <t>swissotel al murooj dubai *****</t>
   </si>
   <si>
@@ -349,9 +277,6 @@
     <t>gulf court hotel business bay 4*</t>
   </si>
   <si>
-    <t>gulf court hotel business bay ****</t>
-  </si>
-  <si>
     <t>canal central hotel business bay *****</t>
   </si>
   <si>
@@ -364,18 +289,12 @@
     <t>swissotel al murooj 5*</t>
   </si>
   <si>
-    <t>swissotel al murooj *****</t>
-  </si>
-  <si>
     <t>swissotel al murooj hotel 5*</t>
   </si>
   <si>
     <t>swissotel al murooj dubai 5*</t>
   </si>
   <si>
-    <t>donatello hotel dubai. ****</t>
-  </si>
-  <si>
     <t>donatello hotel dubai 4*</t>
   </si>
   <si>
@@ -388,27 +307,18 @@
     <t>aloft palm jumeirah 4*</t>
   </si>
   <si>
-    <t>aloft palm jumeirah ****</t>
-  </si>
-  <si>
     <t>aloft the palm jumeirah ****</t>
   </si>
   <si>
     <t>tryp by wyndham dubai 4*</t>
   </si>
   <si>
-    <t>tryp by wyndham dubai ****</t>
-  </si>
-  <si>
     <t>tryp by wyndham dubai barsha heights 4*</t>
   </si>
   <si>
     <t>amwaj rotana jumeirah beach 5*</t>
   </si>
   <si>
-    <t>amwaj rotana jumeirah beach. *****</t>
-  </si>
-  <si>
     <t>amwaj rotana jumeirah beach dubai 5*</t>
   </si>
   <si>
@@ -418,9 +328,6 @@
     <t>amwaj rotana jumeirah beach *****</t>
   </si>
   <si>
-    <t>signature hotel tecom ****</t>
-  </si>
-  <si>
     <t>signature 1 hotel tecom 4*</t>
   </si>
   <si>
@@ -430,18 +337,12 @@
     <t>signature hotel al barsha ****</t>
   </si>
   <si>
-    <t>wyndham dubai marina. ****</t>
-  </si>
-  <si>
     <t>wyndham dubai marina 4*</t>
   </si>
   <si>
     <t>wyndham dubai marina ****</t>
   </si>
   <si>
-    <t>stella di mare dubai marina hotel *****</t>
-  </si>
-  <si>
     <t>stella di mare dubai 5*</t>
   </si>
   <si>
@@ -472,9 +373,6 @@
     <t>ramada hotel &amp; suites by wyndham jbr 4*</t>
   </si>
   <si>
-    <t>the retreat palm dubai. *****</t>
-  </si>
-  <si>
     <t>the retreat palm dubai mgallery by sofitel 5*</t>
   </si>
   <si>
@@ -490,15 +388,9 @@
     <t>hilton dubai the walk 4*</t>
   </si>
   <si>
-    <t>hilton dubai the palm *****</t>
-  </si>
-  <si>
     <t>hilton dubai the palm 5*</t>
   </si>
   <si>
-    <t>towers rotana dubai ****</t>
-  </si>
-  <si>
     <t>towers rotana dubai 4*</t>
   </si>
   <si>
@@ -514,18 +406,12 @@
     <t>gevora hotel 4*</t>
   </si>
   <si>
-    <t>media rotana dubai *****</t>
-  </si>
-  <si>
     <t>media rotana dubai 5*</t>
   </si>
   <si>
     <t>media rotana hotel dubai *****</t>
   </si>
   <si>
-    <t>dukes dubai, a royal hideaway hotel *****</t>
-  </si>
-  <si>
     <t>dukes dubai, a royal hideaway hotel 5*</t>
   </si>
   <si>
@@ -535,15 +421,9 @@
     <t>dukes the palm, a royal hideaway hotel *****</t>
   </si>
   <si>
-    <t>nh dubai the palm ****</t>
-  </si>
-  <si>
     <t>nh dubai the palm 5*</t>
   </si>
   <si>
-    <t>marina byblos. ****</t>
-  </si>
-  <si>
     <t>marina byblos hotel 4*</t>
   </si>
   <si>
@@ -553,9 +433,6 @@
     <t>marina byblos hotel ****</t>
   </si>
   <si>
-    <t>holiday inn dubai-al barsha ****</t>
-  </si>
-  <si>
     <t>holiday inn dubai al barsha 4*</t>
   </si>
   <si>
@@ -565,9 +442,6 @@
     <t>holiday inn dubai - al barsha ****</t>
   </si>
   <si>
-    <t>atana hotel tecom ****</t>
-  </si>
-  <si>
     <t>atana hotel 4*</t>
   </si>
   <si>
@@ -577,18 +451,12 @@
     <t>atana hotel ****</t>
   </si>
   <si>
-    <t>canal central business bay *****</t>
-  </si>
-  <si>
     <t>canal central business bay 5*</t>
   </si>
   <si>
     <t>canal central hotel 5*</t>
   </si>
   <si>
-    <t>rove downtown dubai. ***</t>
-  </si>
-  <si>
     <t>rove downtown dubai 3*</t>
   </si>
   <si>
@@ -598,9 +466,6 @@
     <t>palace downtown dubai *****</t>
   </si>
   <si>
-    <t>holiday inn &amp; suites dubai science park al barsha ****</t>
-  </si>
-  <si>
     <t>holiday inn and suites dubai science park 4*</t>
   </si>
   <si>
@@ -610,9 +475,6 @@
     <t>holiday inn &amp; suites dubai science park 4*</t>
   </si>
   <si>
-    <t>voco monaco dubai*****</t>
-  </si>
-  <si>
     <t>voco dubai 5*</t>
   </si>
   <si>
@@ -622,9 +484,6 @@
     <t>voco dubai*****</t>
   </si>
   <si>
-    <t>blue beach tower *****</t>
-  </si>
-  <si>
     <t>blue beach tower jumeirah beach residenceapartment deluxe</t>
   </si>
   <si>
@@ -643,24 +502,15 @@
     <t>mercure hotel apartmentsapr</t>
   </si>
   <si>
-    <t>the s hotel al barsha ****</t>
-  </si>
-  <si>
     <t>the s hotel al barsha 4*</t>
   </si>
   <si>
     <t>the s hotel al barsha dubai 4*</t>
   </si>
   <si>
-    <t>four points by sheraton bur dubai ****</t>
-  </si>
-  <si>
     <t>four points by sheraton bur dubai 4*</t>
   </si>
   <si>
-    <t>millennium place mirdif ****</t>
-  </si>
-  <si>
     <t>millennium place mirdif 4*</t>
   </si>
   <si>
@@ -673,18 +523,12 @@
     <t>movenpick hotel apartment al mamzar apr</t>
   </si>
   <si>
-    <t>the first collection business bay ****</t>
-  </si>
-  <si>
     <t>the first collection business bay 4*</t>
   </si>
   <si>
     <t>the first collection hotel business bay ****</t>
   </si>
   <si>
-    <t>manzil downtown dubai. ****</t>
-  </si>
-  <si>
     <t>manzil downtown 4*</t>
   </si>
   <si>
@@ -700,15 +544,9 @@
     <t>palazzo versace 5*</t>
   </si>
   <si>
-    <t>ja beach hotel *****</t>
-  </si>
-  <si>
     <t>ja beach hotel 5*</t>
   </si>
   <si>
-    <t>waldorf astoria palm jumeirah. *****</t>
-  </si>
-  <si>
     <t>waldorf astoria dubai palm jumeirah 5*</t>
   </si>
   <si>
@@ -718,9 +556,6 @@
     <t>waldorf astoria palm jumeirah *****</t>
   </si>
   <si>
-    <t>sheraton jumeirah beach resort *****</t>
-  </si>
-  <si>
     <t>sheraton jumeirah beach resort 5*</t>
   </si>
   <si>
@@ -745,9 +580,6 @@
     <t>habtoor grand resort, autograph collection *****</t>
   </si>
   <si>
-    <t>armani hotel dubai. *****</t>
-  </si>
-  <si>
     <t>armani hotel dubai 5*</t>
   </si>
   <si>
@@ -769,9 +601,6 @@
     <t>jumeirah zabeel saray 5*</t>
   </si>
   <si>
-    <t>jumeirah zabeel saray *****</t>
-  </si>
-  <si>
     <t>jumeirah zabeel saray 5* deluxe</t>
   </si>
   <si>
@@ -781,9 +610,6 @@
     <t>rixos premium dubai *****</t>
   </si>
   <si>
-    <t>ja ocean view dubai *****</t>
-  </si>
-  <si>
     <t>ja ocean view hotel 5*</t>
   </si>
   <si>
@@ -802,9 +628,6 @@
     <t>hilton dubai jumeirah 5*</t>
   </si>
   <si>
-    <t>rixos the palm dubai hotel and suites *****</t>
-  </si>
-  <si>
     <t>rixos the palm dubai hotel &amp; suites 5*</t>
   </si>
   <si>
@@ -814,9 +637,6 @@
     <t>atlantis the palm 5*</t>
   </si>
   <si>
-    <t>atlantis the palm dubai *****</t>
-  </si>
-  <si>
     <t>atlantis, the palm 5*</t>
   </si>
   <si>
@@ -826,9 +646,6 @@
     <t>atlantis the palm, dubai 5* deluxe</t>
   </si>
   <si>
-    <t>one &amp; only the palm. *****</t>
-  </si>
-  <si>
     <t>one &amp; only the palm dubai 5*</t>
   </si>
   <si>
@@ -838,9 +655,6 @@
     <t>one &amp; only the palm, dubai 5* deluxe</t>
   </si>
   <si>
-    <t>raffles the palm *****</t>
-  </si>
-  <si>
     <t>raffles the palm 5*</t>
   </si>
   <si>
@@ -850,27 +664,15 @@
     <t>raffles the palm dubai *****</t>
   </si>
   <si>
-    <t>address boulevard *****</t>
-  </si>
-  <si>
-    <t>kempinski central avenue dubai*****</t>
-  </si>
-  <si>
     <t>kempinski central avenue dubai 5*</t>
   </si>
   <si>
-    <t>jumeirah beach hotel *****</t>
-  </si>
-  <si>
     <t>jumeirah beach hotel 5*</t>
   </si>
   <si>
     <t>jumeirah beach hotel 5* deluxe</t>
   </si>
   <si>
-    <t>sofitel the palm. *****</t>
-  </si>
-  <si>
     <t>sofitel the palm 5*</t>
   </si>
   <si>
@@ -883,9 +685,6 @@
     <t>anantara dubai the palm resort 5*</t>
   </si>
   <si>
-    <t>one &amp; only royal mirage - arabian court *****</t>
-  </si>
-  <si>
     <t>one and only royal mirage - arabian court 5*</t>
   </si>
   <si>
@@ -895,9 +694,6 @@
     <t>one &amp; only royal mirage - arabian court 5* deluxe</t>
   </si>
   <si>
-    <t>w dubai mina seyahi *****</t>
-  </si>
-  <si>
     <t>w dubai - mina seyahi 5*</t>
   </si>
   <si>
@@ -907,9 +703,6 @@
     <t>w dubai - mina seyahi *****</t>
   </si>
   <si>
-    <t>the ritz-carlton, dubai *****</t>
-  </si>
-  <si>
     <t>the ritz-carlton, dubai 5*</t>
   </si>
   <si>
@@ -958,9 +751,6 @@
     <t>le royal meridien beach resort &amp; spa 5*</t>
   </si>
   <si>
-    <t>taj exotica resort &amp; spa, the palm *****</t>
-  </si>
-  <si>
     <t>taj exotica resort &amp; spa, the palm, dubai 5*</t>
   </si>
   <si>
@@ -973,9 +763,6 @@
     <t>taj exotica resort &amp; spa, the palm, dubai *****</t>
   </si>
   <si>
-    <t>the oberoi dubai. *****</t>
-  </si>
-  <si>
     <t>the oberoi beach resort al zorah 5*</t>
   </si>
   <si>
@@ -985,33 +772,21 @@
     <t>the oberoi hotel *****</t>
   </si>
   <si>
-    <t>bvlgari resort dubai *****</t>
-  </si>
-  <si>
     <t>bulgari resort dubai 5*</t>
   </si>
   <si>
     <t>bvlgari resort dubai 5*</t>
   </si>
   <si>
-    <t>the st. regis dubai, the palm *****</t>
-  </si>
-  <si>
     <t>the st. regis dubai the palm 5*</t>
   </si>
   <si>
-    <t>mandarin oriental jumeirah dubai *****</t>
-  </si>
-  <si>
     <t>mandarin oriental jumeira, dubai 5*</t>
   </si>
   <si>
     <t>mandarin oriental jumeira dubai 5*</t>
   </si>
   <si>
-    <t>grosvenor house *****</t>
-  </si>
-  <si>
     <t>grosvenor house - tower 1 5*</t>
   </si>
   <si>
@@ -1024,27 +799,18 @@
     <t>grosvenor house dubai *****</t>
   </si>
   <si>
-    <t>banyan tree dubai*****</t>
-  </si>
-  <si>
     <t>banyan tree dubai 5*</t>
   </si>
   <si>
     <t>banyan tree dubai *****</t>
   </si>
   <si>
-    <t>the westin dubai mina seyahi beach resort &amp; marina *****</t>
-  </si>
-  <si>
     <t>the westin dubai mina seyahi beach resort &amp; marina 5*</t>
   </si>
   <si>
     <t>the westin dubai mina seyahi beach resort &amp; spa *****</t>
   </si>
   <si>
-    <t>th8 palm dubai beach resort vignette collection *****</t>
-  </si>
-  <si>
     <t>th8 palm dubai beach resort vignette collection 5*</t>
   </si>
   <si>
@@ -1054,9 +820,6 @@
     <t>jw marriott hotel marina 5*</t>
   </si>
   <si>
-    <t>jw marriott hotel marina*****</t>
-  </si>
-  <si>
     <t>w dubai - the palm *****</t>
   </si>
   <si>
@@ -1108,9 +871,6 @@
     <t>Heritage Hotel, Autograph Collection (ex. Manzil Downtown) 4*</t>
   </si>
   <si>
-    <t>Habtoor Grand Resort, Autograph Collection *****</t>
-  </si>
-  <si>
     <t>Armani Hotel 5*</t>
   </si>
   <si>
@@ -1202,6 +962,120 @@
   </si>
   <si>
     <t>riviera hotel 4*</t>
+  </si>
+  <si>
+    <t>hyatt place dubai/wasl district 4*</t>
+  </si>
+  <si>
+    <t>copthorne hotel dubai. 4*</t>
+  </si>
+  <si>
+    <t>rove dubai marina hotel 3*</t>
+  </si>
+  <si>
+    <t>fortune grand hotel. 4*</t>
+  </si>
+  <si>
+    <t>novotel dubai al barsha. 4*</t>
+  </si>
+  <si>
+    <t>comfort inn hotel. 3*</t>
+  </si>
+  <si>
+    <t>best western plus pearl creek hotel. 4*</t>
+  </si>
+  <si>
+    <t>studio m arabian plaza hotel apartment 3*</t>
+  </si>
+  <si>
+    <t>md hotel dubai 4*</t>
+  </si>
+  <si>
+    <t>grand excelsior bur dubai. 4*</t>
+  </si>
+  <si>
+    <t>al khoory executive. 3*</t>
+  </si>
+  <si>
+    <t>rose rayhaan by rotana. 4*</t>
+  </si>
+  <si>
+    <t>hyatt place dubai/ al rigga 4*</t>
+  </si>
+  <si>
+    <t>delta hotels by marriott, jumeirah beach dubai 4*</t>
+  </si>
+  <si>
+    <t>centara mirage beach dubai 4*</t>
+  </si>
+  <si>
+    <t>donatello hotel dubai. 4*</t>
+  </si>
+  <si>
+    <t>amwaj rotana jumeirah beach. 5*</t>
+  </si>
+  <si>
+    <t>wyndham dubai marina. 4*</t>
+  </si>
+  <si>
+    <t>stella di mare dubai marina hotel 5*</t>
+  </si>
+  <si>
+    <t>the retreat palm dubai. 5*</t>
+  </si>
+  <si>
+    <t>nh dubai the palm 4*</t>
+  </si>
+  <si>
+    <t>marina byblos. 4*</t>
+  </si>
+  <si>
+    <t>atana hotel tecom 4*</t>
+  </si>
+  <si>
+    <t>rove downtown dubai. 3*</t>
+  </si>
+  <si>
+    <t>manzil downtown dubai. 4*</t>
+  </si>
+  <si>
+    <t>waldorf astoria palm jumeirah. 5*</t>
+  </si>
+  <si>
+    <t>Habtoor Grand Resort, Autograph Collection 5*</t>
+  </si>
+  <si>
+    <t>armani hotel dubai. 5*</t>
+  </si>
+  <si>
+    <t>ja ocean view dubai 5*</t>
+  </si>
+  <si>
+    <t>rixos the palm dubai hotel and suites 5*</t>
+  </si>
+  <si>
+    <t>one &amp; only the palm. 5*</t>
+  </si>
+  <si>
+    <t>address boulevard 5*</t>
+  </si>
+  <si>
+    <t>sofitel the palm. 5*</t>
+  </si>
+  <si>
+    <t>anantara dubai the palm resort &amp; spa 5*</t>
+  </si>
+  <si>
+    <t>one &amp; only royal mirage - arabian court 5*</t>
+  </si>
+  <si>
+    <t>the oberoi dubai. 5*</t>
+  </si>
+  <si>
+    <t>the st. regis dubai, the palm 5*</t>
+  </si>
+  <si>
+    <t>mandarin oriental jumeirah dubai 5*</t>
   </si>
 </sst>
 </file>
@@ -1691,10 +1565,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1725,7 +1600,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1742,13 +1617,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>313</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>349</v>
+        <v>270</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>393</v>
+        <v>313</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1759,7 +1634,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -1776,1878 +1651,1878 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>315</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>316</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>317</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>318</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>319</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>43</v>
+        <v>320</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>321</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>322</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>351</v>
+        <v>272</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>375</v>
+        <v>295</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>376</v>
+        <v>296</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>323</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>352</v>
+        <v>273</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>353</v>
+        <v>274</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>374</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>324</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>84</v>
+        <v>325</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>89</v>
+        <v>326</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>92</v>
+        <v>327</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>98</v>
+        <v>328</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>377</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>378</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>117</v>
+        <v>329</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>379</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>128</v>
+        <v>330</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>136</v>
+        <v>331</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>139</v>
+        <v>332</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>354</v>
+        <v>275</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>150</v>
+        <v>333</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>355</v>
+        <v>276</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>390</v>
+        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>356</v>
+        <v>277</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>380</v>
+        <v>300</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>381</v>
+        <v>301</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>171</v>
+        <v>334</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>357</v>
+        <v>278</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>357</v>
+        <v>278</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>382</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>173</v>
+        <v>335</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>181</v>
+        <v>336</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>383</v>
+        <v>303</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>187</v>
+        <v>144</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>188</v>
+        <v>337</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>192</v>
+        <v>149</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>358</v>
+        <v>279</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>197</v>
+        <v>151</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>204</v>
+        <v>157</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>205</v>
+        <v>158</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>359</v>
+        <v>280</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>206</v>
+        <v>159</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>391</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>209</v>
+        <v>161</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>209</v>
+        <v>161</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>384</v>
+        <v>304</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>385</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>212</v>
+        <v>163</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>360</v>
+        <v>281</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>219</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>220</v>
+        <v>338</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>361</v>
+        <v>282</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>221</v>
+        <v>169</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>222</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>225</v>
+        <v>173</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>224</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>226</v>
+        <v>174</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>386</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>228</v>
+        <v>339</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>230</v>
+        <v>176</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>231</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>232</v>
+        <v>178</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>235</v>
+        <v>181</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>238</v>
+        <v>183</v>
       </c>
       <c r="C77" t="s">
-        <v>239</v>
+        <v>184</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>387</v>
+        <v>307</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>241</v>
+        <v>341</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>242</v>
+        <v>186</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>363</v>
+        <v>283</v>
       </c>
       <c r="D78" t="s">
-        <v>242</v>
+        <v>186</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>245</v>
+        <v>189</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>247</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>250</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>252</v>
+        <v>194</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>252</v>
+        <v>195</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>253</v>
+        <v>342</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>254</v>
+        <v>196</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>254</v>
+        <v>196</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>254</v>
+        <v>196</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>255</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>256</v>
+        <v>199</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>259</v>
+        <v>201</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>256</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>260</v>
+        <v>343</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>261</v>
+        <v>202</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>202</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>388</v>
+        <v>308</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>262</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>264</v>
+        <v>206</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>265</v>
+        <v>205</v>
       </c>
       <c r="C86" t="s">
-        <v>266</v>
+        <v>206</v>
       </c>
       <c r="D86" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>267</v>
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>268</v>
+        <v>344</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>269</v>
+        <v>208</v>
       </c>
       <c r="C87" t="s">
-        <v>270</v>
+        <v>209</v>
       </c>
       <c r="D87" t="s">
-        <v>270</v>
+        <v>209</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>272</v>
+        <v>211</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>273</v>
+        <v>211</v>
       </c>
       <c r="C88" t="s">
-        <v>274</v>
+        <v>212</v>
       </c>
       <c r="D88" t="s">
-        <v>273</v>
+        <v>211</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>275</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>276</v>
+        <v>345</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>364</v>
+        <v>284</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>365</v>
+        <v>285</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>366</v>
+        <v>286</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>392</v>
+        <v>312</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>278</v>
+        <v>214</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>367</v>
+        <v>287</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>280</v>
+        <v>215</v>
       </c>
       <c r="C91" t="s">
-        <v>280</v>
+        <v>215</v>
       </c>
       <c r="D91" t="s">
-        <v>280</v>
+        <v>215</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>281</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>282</v>
+        <v>346</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>368</v>
+        <v>288</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>369</v>
+        <v>289</v>
       </c>
       <c r="D92" t="s">
-        <v>283</v>
+        <v>217</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>284</v>
+        <v>347</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>285</v>
+        <v>219</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>370</v>
+        <v>290</v>
       </c>
       <c r="D93" t="s">
-        <v>286</v>
+        <v>220</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>284</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>287</v>
+        <v>348</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>288</v>
+        <v>221</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>289</v>
+        <v>222</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>289</v>
+        <v>222</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>290</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>291</v>
+        <v>225</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>292</v>
+        <v>224</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>292</v>
+        <v>224</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>293</v>
+        <v>225</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>294</v>
+        <v>226</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>295</v>
+        <v>227</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>296</v>
+        <v>227</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>297</v>
+        <v>228</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>296</v>
+        <v>227</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>298</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>299</v>
+        <v>231</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>300</v>
+        <v>231</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>300</v>
+        <v>231</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>300</v>
+        <v>231</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>299</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>301</v>
+        <v>233</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>302</v>
+        <v>233</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>302</v>
+        <v>233</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>302</v>
+        <v>233</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>301</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>303</v>
+        <v>235</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>304</v>
+        <v>235</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>304</v>
+        <v>235</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>304</v>
+        <v>235</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>303</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>306</v>
+        <v>236</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>371</v>
+        <v>291</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>305</v>
+        <v>236</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>307</v>
+        <v>238</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>306</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>308</v>
+        <v>240</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>308</v>
+        <v>239</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>310</v>
+        <v>242</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>311</v>
+        <v>242</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>311</v>
+        <v>242</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>311</v>
+        <v>242</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>310</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>312</v>
+        <v>245</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>313</v>
+        <v>243</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>314</v>
+        <v>244</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>317</v>
+        <v>349</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>319</v>
+        <v>248</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>321</v>
+        <v>251</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>372</v>
+        <v>292</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>322</v>
+        <v>250</v>
       </c>
       <c r="D105" t="s">
-        <v>323</v>
+        <v>251</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>373</v>
+        <v>293</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>325</v>
+        <v>252</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>327</v>
+        <v>253</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>328</v>
+        <v>254</v>
       </c>
       <c r="D107" t="s">
-        <v>327</v>
+        <v>253</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>329</v>
+        <v>257</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>330</v>
+        <v>255</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>331</v>
+        <v>256</v>
       </c>
       <c r="D108" t="s">
-        <v>332</v>
+        <v>257</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>333</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>334</v>
+        <v>259</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>335</v>
+        <v>259</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>335</v>
+        <v>259</v>
       </c>
       <c r="D109" t="s">
-        <v>335</v>
+        <v>259</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>336</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>337</v>
+        <v>261</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>338</v>
+        <v>261</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>338</v>
+        <v>261</v>
       </c>
       <c r="D110" t="s">
-        <v>338</v>
+        <v>261</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>339</v>
+        <v>262</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>340</v>
+        <v>263</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>341</v>
+        <v>263</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>341</v>
+        <v>263</v>
       </c>
       <c r="D111" t="s">
-        <v>342</v>
+        <v>264</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>344</v>
+        <v>265</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>343</v>
+        <v>265</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>343</v>
+        <v>265</v>
       </c>
       <c r="D112" t="s">
-        <v>343</v>
+        <v>265</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>345</v>
+        <v>268</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>346</v>
+        <v>267</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>345</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
       <c r="B114" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
       <c r="C114" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
       <c r="D114" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
       <c r="E114" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A2:E2 A24:E25 A60:E61 A62:D62 A69:D69 A105:A106 A107:C109 A113:E113 A68:D68 A4:E6 A3 D3:E3 A15:E15 A14 C14:D14 A22:C22 A20:A21 C20:D20 A23 D23 A49:E50 A47 C47:E47 A48:B48 D48:E48 A52:E52 A51:B51 D51 A54:E54 A53:B53 E53 A57:E58 A56 C56 A64:D64 A63 C63:E63 A66:E66 A65:B65 D65 A72:E72 A70:A71 C70:C71 A79:E84 B77 A78:B78 A91:B91 A89 A90:B90 A94:E99 A92 A93:B93 A101:E104 A100 C100:E100 C105 C106 A114:E114 A12:E12 A11:C11 E11 A9:E10 A8:D8 A13:D13 A17:E17 A16:D16 A27:E33 A26:D26 A19:E19 A18:C18 E18 E22 A35:E36 A38:E41 A37:D37 A43:E46 A42:D42 A55:C55 E55 A59:C59 E59 A67:C67 E70:E71 A74:E76 A73:D73 A85:B88 A110:C112 A7:B7 D7:E7" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:E1 B2:E2 B25:E25 B61:E61 B62:D62 B69:D69 B109:C109 B113:E113 B68:D68 B6:E6 D3:E3 B15:E15 C14:D14 B22:C22 C20:D20 D23 B50:E50 C47:E47 B48 D48:E48 B52:E52 B51 D51 B54:E54 B53 E53 B58:E58 C56 B64:D64 C63:E63 B66:E66 B65 D65 B72:E72 C70:C71 B84:E84 B77 B78 B91 B90 B99:E99 B93 B104:E104 C100:E100 C105 C106 A114:E114 B12:E12 B11:C11 E11 B10:E10 B8 B13:D13 B17:E17 B16:D16 B33:E33 B26:D26 B19:E19 B18:C18 E18 E22 B36:E36 B41:E41 B37:D37 B46:E46 B42:D42 B55:C55 E55 B59:C59 E59 B67:C67 E70:E71 B76:E76 B73:D73 B88 B112:C112 B7 D7:E7 D8 B4:E4 B5:E5 B9:E9 B24:E24 B27:E27 B28:E28 B29:E29 B30:E30 B31:E31 B32:E32 B35:E35 B38:E38 B39:E39 B40:E40 B43:E43 B44:E44 B45:E45 B49:E49 B57:E57 B60:E60 B74:E74 B75:E75 B79:E79 B80:E80 B81:E81 B82:E82 B83:E83 B85 B86 B87 B94:E94 B95:E95 B96:E96 B97:E97 B98:E98 B101:E101 B102:E102 B103:E103 B107:C107 B108:C108 B110:C110 B111:C111" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added extra normalization steps for hotelnames from the hotelmappings; pageload timeout set to 10s, better normalization logic for hotelnames, smarter room type normalization logic, new hotelmappings and templates
</commit_message>
<xml_diff>
--- a/puppeteer-server/assets/UAE_MatchedHotels.xlsx
+++ b/puppeteer-server/assets/UAE_MatchedHotels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asimov\Desktop\develop\webscraper\puppeteer-server\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DA7C3C-9F34-493C-889F-B75A1C4D83F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFB22BF-613E-4064-9CF2-E0AA6AE73B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="381">
   <si>
     <t>Online Centrum</t>
   </si>
@@ -493,15 +493,6 @@
     <t>blue beach tower 5*</t>
   </si>
   <si>
-    <t>mercure hotel apartmentsaprt</t>
-  </si>
-  <si>
-    <t>mercure hotel apartments dubai barsha heights apartment</t>
-  </si>
-  <si>
-    <t>mercure hotel apartmentsapr</t>
-  </si>
-  <si>
     <t>the s hotel al barsha 4*</t>
   </si>
   <si>
@@ -829,18 +820,12 @@
     <t>w dubai - the palm 5*</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Riviera Hotel Dubai 4*</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>MD Hotel By Gewan formerly Cassells 4*</t>
-  </si>
-  <si>
     <t>Rose Park Al Barsha 4*</t>
   </si>
   <si>
@@ -862,9 +847,6 @@
     <t>Voco Monaco Dubai (ex. Cote D'Azur Hotel Monaco) 5*</t>
   </si>
   <si>
-    <t>Mercure Hotel Suites &amp; Apartments, Barsha Heights 4*</t>
-  </si>
-  <si>
     <t>The First Collection Hotel Business Bay 4*</t>
   </si>
   <si>
@@ -955,9 +937,6 @@
     <t>HILTON DUBAI PALM JUMEIRAH *****</t>
   </si>
   <si>
-    <t>MERCURE HOTELS SUITES APARTMENTS, BARSHA HEIGHTS Hotel Apartments Standard</t>
-  </si>
-  <si>
     <t>KEMPINSKI THE BOULEVARD DUBAI *****</t>
   </si>
   <si>
@@ -1006,9 +985,6 @@
     <t>delta hotels by marriott, jumeirah beach dubai 4*</t>
   </si>
   <si>
-    <t>centara mirage beach dubai 4*</t>
-  </si>
-  <si>
     <t>donatello hotel dubai. 4*</t>
   </si>
   <si>
@@ -1076,6 +1052,117 @@
   </si>
   <si>
     <t>mandarin oriental jumeirah dubai 5*</t>
+  </si>
+  <si>
+    <t>Signature Hotel Al Barsha 4*</t>
+  </si>
+  <si>
+    <t>SIGNATURE HOTEL AL BARSHA ****</t>
+  </si>
+  <si>
+    <t>Golden Tulip Deira 4*</t>
+  </si>
+  <si>
+    <t>Golden Tulip Deira Hotel 4*</t>
+  </si>
+  <si>
+    <t>GOLDEN TULIP DEIRA 4*</t>
+  </si>
+  <si>
+    <t>GOLDEN TULIP DEIRA HOTEL ****</t>
+  </si>
+  <si>
+    <t>Millennium Plaza Downtown Hotel 5*</t>
+  </si>
+  <si>
+    <t>MILLENNIUM PLAZA DOWNTOWN 5*</t>
+  </si>
+  <si>
+    <t>MILLENNIUM PLAZA HOTEL DUBAI *****</t>
+  </si>
+  <si>
+    <t>Rose Plaza Hotel Al Barsha 3*</t>
+  </si>
+  <si>
+    <t>ROSE PLAZA HOTEL - AL BARSHA ***</t>
+  </si>
+  <si>
+    <t>Signature Hotel Apartments &amp; Spa Marina 4</t>
+  </si>
+  <si>
+    <t>Signature Hotel Apartments Marina APR</t>
+  </si>
+  <si>
+    <t>SIGNATURE HOTEL APARTMENTS &amp; SPA, MARINA Hotel Apartments Deluxe</t>
+  </si>
+  <si>
+    <t>Dusit D2 Kenz Hotel Dubai 4*</t>
+  </si>
+  <si>
+    <t>DUSIT D2 KENZ HOTEL DUBAI ****</t>
+  </si>
+  <si>
+    <t>Royal Hotel 3*</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express Internet City 3*</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express Dubai Internet City 3*</t>
+  </si>
+  <si>
+    <t>HOLIDAY INN EXPRESS DUBAI INTERNET CITY ***</t>
+  </si>
+  <si>
+    <t>Al Khoory Atrium Hotel 4*</t>
+  </si>
+  <si>
+    <t>Al Khoory Atrium Hotel - Al Barsha 4*</t>
+  </si>
+  <si>
+    <t>AL KHOORY ATRIUM HOTEL ****</t>
+  </si>
+  <si>
+    <t>Rixos Bab Al Bahr 5*</t>
+  </si>
+  <si>
+    <t>RIXOS BAB AL BAHR *****</t>
+  </si>
+  <si>
+    <t>Signature Hotel Apartments &amp; Spa Marina Aprt</t>
+  </si>
+  <si>
+    <t>Al Khoory Atrium 4*</t>
+  </si>
+  <si>
+    <t>Mercure Hotel Apartments Dubai Barsha Heights APARTMENT</t>
+  </si>
+  <si>
+    <t>MERCURE HOTELS SUITES &amp; APARTMENTS, BARSHA HEIGHTS Hotel Apartments</t>
+  </si>
+  <si>
+    <t>Mercure Hotel Apartments APR</t>
+  </si>
+  <si>
+    <t>Mercure Hotel Apartments Aprt</t>
+  </si>
+  <si>
+    <t>Holiday Inn Dubai al-Maktoum Airport, an IHG Hotel 4*</t>
+  </si>
+  <si>
+    <t>Holiday Inn Dubai Al Maktoum Airport 4*</t>
+  </si>
+  <si>
+    <t>Md Hotel 4*</t>
+  </si>
+  <si>
+    <t>Millennium Al Barsha Mall Of The Emirates 4*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signature Hotel Apartments &amp; Spa Marina APARTMENT             </t>
+  </si>
+  <si>
+    <t>Hyatt Place Baniyas Square 4*</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1226,6 +1313,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1566,10 +1659,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1578,10 +1671,10 @@
     <col min="2" max="2" width="65.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1617,13 +1710,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1651,7 +1744,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -1668,7 +1761,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
@@ -1714,12 +1807,12 @@
         <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
@@ -1753,7 +1846,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
@@ -1762,7 +1855,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>28</v>
@@ -1787,7 +1880,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>32</v>
@@ -1799,15 +1892,15 @@
         <v>33</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>34</v>
@@ -1816,12 +1909,12 @@
         <v>34</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>35</v>
@@ -1850,7 +1943,7 @@
         <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1881,7 +1974,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>45</v>
@@ -1906,10 +1999,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>48</v>
@@ -1918,29 +2011,29 @@
         <v>49</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>272</v>
+        <v>377</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
@@ -1949,7 +2042,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>52</v>
@@ -1960,16 +2053,16 @@
         <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1991,7 +2084,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>57</v>
@@ -2020,7 +2113,7 @@
         <v>62</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2042,7 +2135,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>65</v>
@@ -2062,10 +2155,10 @@
         <v>67</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>380</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>380</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>67</v>
@@ -2076,7 +2169,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>69</v>
@@ -2093,7 +2186,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>71</v>
@@ -2125,9 +2218,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>328</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>76</v>
@@ -2156,7 +2249,7 @@
         <v>78</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2207,7 +2300,7 @@
         <v>84</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2215,7 +2308,7 @@
         <v>86</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>86</v>
+        <v>378</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>86</v>
@@ -2246,7 +2339,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>91</v>
@@ -2292,12 +2385,12 @@
         <v>96</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>98</v>
@@ -2331,7 +2424,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>105</v>
@@ -2348,7 +2441,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>107</v>
@@ -2368,7 +2461,7 @@
         <v>111</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>112</v>
@@ -2388,7 +2481,7 @@
         <v>115</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>116</v>
@@ -2399,7 +2492,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>117</v>
@@ -2439,13 +2532,13 @@
         <v>122</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2473,10 +2566,10 @@
         <v>127</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>126</v>
@@ -2510,7 +2603,7 @@
         <v>131</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>132</v>
@@ -2518,24 +2611,24 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>134</v>
@@ -2569,7 +2662,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>140</v>
@@ -2578,7 +2671,7 @@
         <v>141</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>142</v>
@@ -2603,7 +2696,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>145</v>
@@ -2632,7 +2725,7 @@
         <v>150</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2640,7 +2733,7 @@
         <v>152</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>151</v>
@@ -2666,7 +2759,7 @@
         <v>156</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2674,118 +2767,118 @@
         <v>157</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>280</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>311</v>
+        <v>158</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>40</v>
+        <v>159</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>305</v>
+        <v>160</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>163</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>282</v>
+        <v>168</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -2793,7 +2886,7 @@
         <v>171</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>171</v>
@@ -2801,30 +2894,30 @@
       <c r="D72" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>172</v>
+      <c r="E72" s="5" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>339</v>
+        <v>175</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>175</v>
@@ -2833,10 +2926,10 @@
         <v>175</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2847,188 +2940,188 @@
         <v>178</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>178</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" t="s">
         <v>181</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
-        <v>340</v>
+      <c r="A77" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C77" t="s">
-        <v>184</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>185</v>
+      <c r="C77" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D77" t="s">
+        <v>183</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>341</v>
+        <v>185</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="D78" t="s">
-        <v>186</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>271</v>
+      <c r="E78" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>342</v>
+        <v>196</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>199</v>
+        <v>335</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" t="s">
+        <v>199</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E84" s="9" t="s">
         <v>200</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>343</v>
+        <v>203</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C85" t="s">
-        <v>202</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>308</v>
+        <v>203</v>
+      </c>
+      <c r="D85" t="s">
+        <v>201</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>206</v>
+        <v>336</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>205</v>
@@ -3037,7 +3130,7 @@
         <v>206</v>
       </c>
       <c r="D86" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>207</v>
@@ -3045,7 +3138,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>344</v>
+        <v>208</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>208</v>
@@ -3054,7 +3147,7 @@
         <v>209</v>
       </c>
       <c r="D87" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>210</v>
@@ -3062,115 +3155,115 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C88" t="s">
-        <v>212</v>
-      </c>
-      <c r="D88" t="s">
-        <v>211</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>213</v>
+        <v>337</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>284</v>
+        <v>211</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>312</v>
+        <v>281</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>271</v>
+        <v>212</v>
+      </c>
+      <c r="C90" t="s">
+        <v>212</v>
+      </c>
+      <c r="D90" t="s">
+        <v>212</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C91" t="s">
-        <v>215</v>
+        <v>338</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="D91" t="s">
-        <v>215</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>288</v>
+        <v>339</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D92" t="s">
         <v>217</v>
       </c>
-      <c r="E92" s="5" t="s">
-        <v>309</v>
+      <c r="E92" s="9" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="D93" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>348</v>
+        <v>222</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>221</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>222</v>
@@ -3181,16 +3274,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>224</v>
       </c>
       <c r="C95" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>226</v>
@@ -3198,64 +3291,64 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>228</v>
       </c>
       <c r="D96" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>235</v>
@@ -3266,36 +3359,36 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E100" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -3303,24 +3396,24 @@
         <v>242</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>242</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>245</v>
+        <v>341</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>244</v>
@@ -3334,138 +3427,138 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" t="s">
         <v>248</v>
       </c>
-      <c r="E104" s="3" t="s">
-        <v>249</v>
+      <c r="E104" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D105" t="s">
-        <v>251</v>
+        <v>249</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>293</v>
+        <v>343</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>271</v>
+        <v>251</v>
+      </c>
+      <c r="D106" t="s">
+        <v>250</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>351</v>
+        <v>254</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="D107" t="s">
         <v>254</v>
       </c>
-      <c r="D107" t="s">
-        <v>253</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>271</v>
+      <c r="E107" s="9" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>256</v>
       </c>
       <c r="D108" t="s">
+        <v>256</v>
+      </c>
+      <c r="E108" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" t="s">
+        <v>258</v>
+      </c>
+      <c r="E109" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="D109" t="s">
-        <v>259</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D110" t="s">
         <v>261</v>
       </c>
-      <c r="E110" s="9" t="s">
-        <v>262</v>
+      <c r="E110" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D111" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -3473,56 +3566,211 @@
         <v>265</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E112" s="4" t="s">
-        <v>271</v>
+      <c r="E112" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>266</v>
+      <c r="A113" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="D113" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>269</v>
-      </c>
-      <c r="B114" t="s">
-        <v>269</v>
-      </c>
-      <c r="C114" t="s">
-        <v>269</v>
-      </c>
-      <c r="D114" t="s">
-        <v>269</v>
-      </c>
-      <c r="E114" t="s">
-        <v>269</v>
+      <c r="A114" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="D114" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="D115" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="D116" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="D117" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="E117" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D118" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="E118" s="13" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="B119" s="13"/>
+      <c r="C119" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="D119" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="E119" s="15"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="B120" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="D120" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B122" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="D122" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="B123" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="D123" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="E123" s="17" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>375</v>
+      </c>
+      <c r="B124" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:E1 B2:E2 B25:E25 B61:E61 B62:D62 B69:D69 B109:C109 B113:E113 B68:D68 B6:E6 D3:E3 B15:E15 C14:D14 B22:C22 C20:D20 D23 B50:E50 C47:E47 B48 D48:E48 B52:E52 B51 D51 B54:E54 B53 E53 B58:E58 C56 B64:D64 C63:E63 B66:E66 B65 D65 B72:E72 C70:C71 B84:E84 B77 B78 B91 B90 B99:E99 B93 B104:E104 C100:E100 C105 C106 A114:E114 B12:E12 B11:C11 E11 B10:E10 B8 B13:D13 B17:E17 B16:D16 B33:E33 B26:D26 B19:E19 B18:C18 E18 E22 B36:E36 B41:E41 B37:D37 B46:E46 B42:D42 B55:C55 E55 B59:C59 E59 B67:C67 E70:E71 B76:E76 B73:D73 B88 B112:C112 B7 D7:E7 D8 B4:E4 B5:E5 B9:E9 B24:E24 B27:E27 B28:E28 B29:E29 B30:E30 B31:E31 B32:E32 B35:E35 B38:E38 B39:E39 B40:E40 B43:E43 B44:E44 B45:E45 B49:E49 B57:E57 B60:E60 B74:E74 B75:E75 B79:E79 B80:E80 B81:E81 B82:E82 B83:E83 B85 B86 B87 B94:E94 B95:E95 B96:E96 B97:E97 B98:E98 B101:E101 B102:E102 B103:E103 B107:C107 B108:C108 B110:C110 B111:C111" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:E1 B2:E2 B25:E25 B61:E61 B62:D62 B68:D68 B108:C108 B112:E112 B67:D67 B6:E6 D3:E3 B15:E15 C14:D14 B22:C22 C20:D20 D23 B50:E50 C47:E47 B48 D48:E48 B52:E52 B51 D51 B54:E54 B53 E53 B58:E58 C56 B64:D64 C63:E63 B65:E65 B71:E71 C69:C70 B83:E83 B76 B77 B90 B89 B98:E98 B92 B103:E103 C99:E99 C104 C105 B12:E12 B11:C11 E11 B10:E10 B8 B13:D13 B17:E17 B16:D16 B33:E33 B26:D26 B19:E19 B18:C18 E18 E22 B36:E36 B41:E41 B37:D37 B46:E46 B42:D42 B55:C55 E55 B59:C59 E59 B66:C66 E69:E70 B75:E75 B72:D72 B87 B111:C111 B7 D7:E7 D8 B4:E4 C5:E5 B9:E9 B24:E24 B27:E27 B28:E28 D29:E29 B30:E30 B31:E31 B32:E32 B35:E35 C38:E38 B39:E39 B40:E40 B43:E43 B44:E44 B45:E45 B49:E49 B57:E57 B60:E60 B73:E73 B74:E74 B78:E78 B79:E79 B80:E80 B81:E81 B82:E82 B84 B85 B86 B93:E93 B94:E94 B95:E95 B96:E96 B97:E97 B100:E100 B101:E101 B102:E102 B106:C106 B107:C107 B109:C109 B110:C110" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>